<commit_message>
Translate table header to Russian
</commit_message>
<xml_diff>
--- a/lab01/Квартиры.xlsx
+++ b/lab01/Квартиры.xlsx
@@ -16,28 +16,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="185">
   <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>subtitle</t>
-  </si>
-  <si>
-    <t>special_geo</t>
-  </si>
-  <si>
-    <t>housing</t>
-  </si>
-  <si>
-    <t>labels</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>price_per_meter</t>
-  </si>
-  <si>
-    <t>agent</t>
+    <t>Название</t>
+  </si>
+  <si>
+    <t>Квартира</t>
+  </si>
+  <si>
+    <t>Расположение</t>
+  </si>
+  <si>
+    <t>Жилой комплекс</t>
+  </si>
+  <si>
+    <t>Адрес</t>
+  </si>
+  <si>
+    <t>Цена</t>
+  </si>
+  <si>
+    <t>Цена за м²</t>
+  </si>
+  <si>
+    <t>Застройщик</t>
   </si>
   <si>
     <t>Квартира с видом на Москву-реку</t>

</xml_diff>